<commit_message>
update R and RStudio
Packages updated, code bugs fixed, and lock file updated
</commit_message>
<xml_diff>
--- a/Paper/paper_tables.xlsx
+++ b/Paper/paper_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hussein/Documents/Code Repos/Bicycle-Network-Optimization/Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F8E836-A6FA-0546-9741-4ADEB1B85CE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA53D5B-297A-0541-99A3-50FE050864F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14260" activeTab="4" xr2:uid="{4D616363-E8C1-A242-9017-079B0D356725}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14260" activeTab="1" xr2:uid="{4D616363-E8C1-A242-9017-079B0D356725}"/>
   </bookViews>
   <sheets>
     <sheet name="Road Types" sheetId="2" r:id="rId1"/>
@@ -37,12 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="102">
   <si>
     <t>OSM Road Type</t>
-  </si>
-  <si>
-    <t>Weight</t>
   </si>
   <si>
     <t xml:space="preserve">OSM Road Type </t>
@@ -474,6 +471,18 @@
   <si>
     <t>Postponed decision</t>
   </si>
+  <si>
+    <t>Weighting Profile</t>
+  </si>
+  <si>
+    <t>Weighted</t>
+  </si>
+  <si>
+    <t>Unweighted</t>
+  </si>
+  <si>
+    <t>Weighted_2</t>
+  </si>
 </sst>
 </file>
 
@@ -482,7 +491,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -571,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -587,24 +596,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -639,6 +630,33 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -960,124 +978,124 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="21"/>
+    </row>
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="34">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:3" ht="34">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="51">
-      <c r="A10" s="2" t="s">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="34">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="34">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -1092,118 +1110,204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6313F688-6078-B941-87F8-70A10AB0124F}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="28"/>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="C6" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="D6" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="D9" s="3">
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="3">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D12" s="3">
         <v>0</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B12">
-    <sortCondition descending="1" ref="B2:B12"/>
-    <sortCondition ref="A2:A12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B13">
+    <sortCondition descending="1" ref="B3:B13"/>
+    <sortCondition ref="A3:A13"/>
   </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1216,43 +1320,43 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="4" max="5" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="B2" s="12"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="25"/>
       <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="11" t="s">
-        <v>28</v>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="B4" s="1">
         <v>100</v>
@@ -1261,14 +1365,14 @@
         <v>0.65</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="11"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="24"/>
       <c r="B5" s="1">
         <v>200</v>
       </c>
@@ -1276,15 +1380,15 @@
         <v>0.82</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="B6" s="1">
         <v>100</v>
@@ -1293,14 +1397,14 @@
         <v>0.68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="11"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="24"/>
       <c r="B7" s="1">
         <v>200</v>
       </c>
@@ -1308,15 +1412,15 @@
         <v>0.85</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="11" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="B8" s="1">
         <v>100</v>
@@ -1325,14 +1429,14 @@
         <v>0.67500000000000004</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="11"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="24"/>
       <c r="B9" s="1">
         <v>200</v>
       </c>
@@ -1340,13 +1444,13 @@
         <v>0.83</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1374,23 +1478,23 @@
       <selection activeCell="C9" sqref="C9:G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1401,7 +1505,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1412,7 +1516,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1423,7 +1527,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1443,11 +1547,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724C1A5C-F0B1-134E-901B-FE3DBFDD382D}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
@@ -1456,276 +1560,276 @@
     <col min="5" max="5" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" thickBot="1">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="14" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" ht="128" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>43935</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>43941</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="106" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>43952</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="121" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>43971</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="76" thickBot="1">
-      <c r="A2" s="15">
-        <v>43927</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" ht="128" customHeight="1" thickBot="1">
-      <c r="A3" s="15">
-        <v>43935</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="C6" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="16" t="s">
+      <c r="D6" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>43973</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="46" thickBot="1">
-      <c r="A4" s="15">
-        <v>43941</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="16" t="s">
+      <c r="C7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>43974</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="13">
+        <v>43979</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="105" x14ac:dyDescent="0.2">
+      <c r="A10" s="13">
+        <v>43987</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16">
+        <v>43985</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="115" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>43994</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D12" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="115" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>44000</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="91" thickBot="1">
-      <c r="A5" s="15">
-        <v>43952</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="76" thickBot="1">
-      <c r="A6" s="15">
-        <v>43971</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="46" thickBot="1">
-      <c r="A7" s="15">
-        <v>43973</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="17" t="s">
+      <c r="C13" s="14"/>
+      <c r="D13" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A14" s="13">
+        <v>44012</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="31" thickBot="1">
-      <c r="A8" s="15">
-        <v>43974</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="19">
-        <v>43979</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="75">
-      <c r="A10" s="19">
-        <v>43987</v>
-      </c>
-      <c r="B10" s="20" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="16">
+        <v>44027</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="75" customHeight="1">
-      <c r="A11" s="22">
-        <v>43985</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="115" customHeight="1" thickBot="1">
-      <c r="A12" s="15">
-        <v>43994</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="20" t="s">
+      <c r="E15" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="16">
+        <v>44043</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="1:5" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="16">
+        <v>44050</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="115" customHeight="1" thickBot="1">
-      <c r="A13" s="15">
-        <v>44000</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="60">
-      <c r="A14" s="19">
-        <v>44012</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-    </row>
-    <row r="15" spans="1:5" ht="70" customHeight="1">
-      <c r="A15" s="22">
-        <v>44027</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="22">
-        <v>44043</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-    </row>
-    <row r="17" spans="1:5" ht="47" customHeight="1">
-      <c r="A17" s="22">
-        <v>44050</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="24" t="s">
+      <c r="D17" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="24"/>
+      <c r="E17" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>